<commit_message>
Update xlxs file to change expected answer which caused false bug
</commit_message>
<xml_diff>
--- a/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test1_Frozen/QuerySet1.xlsx
+++ b/AutomaticProjectTesting_Aug2015_VS2015/EmptyGeneralTesting/Release/Test1_Frozen/QuerySet1.xlsx
@@ -1416,9 +1416,6 @@
     <t>Parent Excessive Arguments NoResult</t>
   </si>
   <si>
-    <t xml:space="preserve"> Select s such that Parent ( 1 , 2 )</t>
-  </si>
-  <si>
     <t>Select s suchthat Parent(1, 2)</t>
   </si>
   <si>
@@ -1428,9 +1425,6 @@
     <t>stmt Parent;</t>
   </si>
   <si>
-    <t>Select Parent such that Parent(1, 2)</t>
-  </si>
-  <si>
     <t>Select SingleSynonym Stmt Parent IntInt ParentKeywordAsSynonym HaveResult</t>
   </si>
   <si>
@@ -1488,12 +1482,6 @@
     <t>Select SingleSynonym Stmt Parent UnderscoreSynonym HaveResult</t>
   </si>
   <si>
-    <t>stmt s, Parent;</t>
-  </si>
-  <si>
-    <t>Select s such that Parent(Parent, 5)</t>
-  </si>
-  <si>
     <t>Select SingleSynonym Stmt Parent SynonymInt ParentKeywordAsSynontm As RelationArg HaveResult</t>
   </si>
   <si>
@@ -1650,9 +1638,6 @@
     <t>Select w such that Parent(1, _)</t>
   </si>
   <si>
-    <t>Select SingleSynonym While Parent IntUnderscore HaveResult</t>
-  </si>
-  <si>
     <t>Select w such that Parent(_, w)</t>
   </si>
   <si>
@@ -1725,9 +1710,6 @@
     <t>Select SingleSynonym Stmt Parent IntSynonym And Parent IntSynonym BothRelationSameSynonym NoResult</t>
   </si>
   <si>
-    <t>Select s1 such that Parent(1, s2) and Parent(2, s3)</t>
-  </si>
-  <si>
     <t>Select SingleSynonym Stmt Parent IntSynonym And Parent IntSynonym BothRelationDiffSynonym HaveResult</t>
   </si>
   <si>
@@ -1794,21 +1776,12 @@
     <t>Select s1 such that Parent(s1, s2) and Parent(s2, s3)</t>
   </si>
   <si>
-    <t>Select SingleSynonym Stmt Parent SynonymSynonym And Parent SynonymSynonym Chain GetFirst HaveResult</t>
-  </si>
-  <si>
     <t>Select s2 such that Parent(s1, s2) and Parent(s2, s3)</t>
   </si>
   <si>
-    <t>Select SingleSynonym Stmt Parent SynonymSynonym And Parent SynonymSynonym Chain GetMiddle HaveResult</t>
-  </si>
-  <si>
     <t>Select s3 such that Parent(s1, s2) and Parent(s2, s3)</t>
   </si>
   <si>
-    <t>Select SingleSynonym Stmt Parent SynonymSynonym And Parent SynonymSynonym Chain GetLast HaveResult</t>
-  </si>
-  <si>
     <t>Select s1 such that Parent(s1, s3) and Parent(s2, s3)</t>
   </si>
   <si>
@@ -1855,6 +1828,33 @@
   </si>
   <si>
     <t>Select Boolean NoDeclaration InvalidQuery Invalid StartOfQuery False</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Select s such that Parent ( 3 , 4 )</t>
+  </si>
+  <si>
+    <t>Select Parent such that Parent(3, 4)</t>
+  </si>
+  <si>
+    <t>Select Parent such that Parent(Parent, 5)</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym While Parent IntUnderscore NoResult</t>
+  </si>
+  <si>
+    <t>Select s1 such that Parent(3, s2) and Parent(3, s3)</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Parent SynonymSynonym And Parent SynonymSynonym Chain GetFirst NoResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Parent SynonymSynonym And Parent SynonymSynonym Chain GetMiddle NoResult</t>
+  </si>
+  <si>
+    <t>Select SingleSynonym Stmt Parent SynonymSynonym And Parent SynonymSynonym Chain GetLast NoResult</t>
   </si>
 </sst>
 </file>
@@ -2211,8 +2211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3B02F3-8668-4835-B18A-9EFEA275CE21}">
   <dimension ref="A1:E294"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C294" sqref="C294"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="E295" sqref="E295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2567,16 +2567,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>609</v>
+        <v>600</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>261</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>603</v>
+        <v>594</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>610</v>
+        <v>601</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2587,13 +2587,13 @@
         <v>5</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>607</v>
+        <v>598</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>603</v>
+        <v>594</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>608</v>
+        <v>599</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2601,13 +2601,13 @@
         <v>22</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>604</v>
+        <v>595</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>603</v>
+        <v>594</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>611</v>
+        <v>602</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2621,7 +2621,7 @@
         <v>261</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>603</v>
+        <v>594</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>263</v>
@@ -2635,13 +2635,13 @@
         <v>5</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>605</v>
+        <v>596</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>603</v>
+        <v>594</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>606</v>
+        <v>597</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -6000,14 +6000,14 @@
       <c r="B223" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C223" s="4" t="s">
-        <v>465</v>
+      <c r="C223" s="10" t="s">
+        <v>603</v>
       </c>
       <c r="D223" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E223" s="4" t="s">
-        <v>600</v>
+        <v>591</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
@@ -6018,7 +6018,7 @@
         <v>5</v>
       </c>
       <c r="C224" s="4" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D224" s="7" t="s">
         <v>34</v>
@@ -6035,7 +6035,7 @@
         <v>5</v>
       </c>
       <c r="C225" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D225" s="7" t="s">
         <v>34</v>
@@ -6049,16 +6049,16 @@
         <v>225</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>468</v>
-      </c>
-      <c r="C226" s="4" t="s">
-        <v>469</v>
+        <v>467</v>
+      </c>
+      <c r="C226" s="10" t="s">
+        <v>604</v>
       </c>
       <c r="D226" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E226" s="4" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
@@ -6069,7 +6069,7 @@
         <v>5</v>
       </c>
       <c r="C227" s="4" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D227" s="7" t="s">
         <v>34</v>
@@ -6086,7 +6086,7 @@
         <v>5</v>
       </c>
       <c r="C228" s="4" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D228" s="7" t="s">
         <v>34</v>
@@ -6103,13 +6103,13 @@
         <v>5</v>
       </c>
       <c r="C229" s="4" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D229" s="7" t="s">
         <v>34</v>
       </c>
       <c r="E229" s="4" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
@@ -6120,13 +6120,13 @@
         <v>5</v>
       </c>
       <c r="C230" s="4" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D230" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E230" s="4" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
@@ -6137,13 +6137,13 @@
         <v>5</v>
       </c>
       <c r="C231" s="4" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D231" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E231" s="4" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
@@ -6154,13 +6154,13 @@
         <v>5</v>
       </c>
       <c r="C232" s="4" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D232" s="6" t="s">
-        <v>601</v>
+        <v>592</v>
       </c>
       <c r="E232" s="4" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
@@ -6171,13 +6171,13 @@
         <v>5</v>
       </c>
       <c r="C233" s="4" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D233" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E233" s="4" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
@@ -6188,13 +6188,13 @@
         <v>5</v>
       </c>
       <c r="C234" s="4" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D234" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E234" s="4" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
@@ -6205,13 +6205,13 @@
         <v>5</v>
       </c>
       <c r="C235" s="4" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D235" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E235" s="4" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
@@ -6222,30 +6222,30 @@
         <v>5</v>
       </c>
       <c r="C236" s="4" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D236" s="6" t="s">
-        <v>601</v>
+        <v>592</v>
       </c>
       <c r="E236" s="4" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="5">
         <v>236</v>
       </c>
-      <c r="B237" s="4" t="s">
-        <v>489</v>
-      </c>
-      <c r="C237" s="4" t="s">
-        <v>490</v>
-      </c>
-      <c r="D237" s="6" t="s">
-        <v>34</v>
+      <c r="B237" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="C237" s="10" t="s">
+        <v>605</v>
+      </c>
+      <c r="D237" s="9" t="s">
+        <v>606</v>
       </c>
       <c r="E237" s="4" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
@@ -6256,13 +6256,13 @@
         <v>5</v>
       </c>
       <c r="C238" s="4" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="D238" s="8">
         <v>3</v>
       </c>
       <c r="E238" s="4" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
@@ -6273,13 +6273,13 @@
         <v>5</v>
       </c>
       <c r="C239" s="4" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="D239" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E239" s="4" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
@@ -6290,13 +6290,13 @@
         <v>5</v>
       </c>
       <c r="C240" s="4" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="D240" s="8">
         <v>3</v>
       </c>
       <c r="E240" s="4" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
@@ -6307,13 +6307,13 @@
         <v>27</v>
       </c>
       <c r="C241" s="4" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="D241" s="8">
         <v>3</v>
       </c>
       <c r="E241" s="4" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
@@ -6324,13 +6324,13 @@
         <v>27</v>
       </c>
       <c r="C242" s="4" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="D242" s="6" t="s">
-        <v>601</v>
+        <v>592</v>
       </c>
       <c r="E242" s="4" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
@@ -6341,13 +6341,13 @@
         <v>5</v>
       </c>
       <c r="C243" s="4" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="D243" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E243" s="4" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
@@ -6358,13 +6358,13 @@
         <v>8</v>
       </c>
       <c r="C244" s="4" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="D244" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E244" s="4" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
@@ -6375,13 +6375,13 @@
         <v>8</v>
       </c>
       <c r="C245" s="4" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="D245" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E245" s="4" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -6392,13 +6392,13 @@
         <v>8</v>
       </c>
       <c r="C246" s="4" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="D246" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E246" s="4" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
@@ -6409,13 +6409,13 @@
         <v>137</v>
       </c>
       <c r="C247" s="4" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="D247" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E247" s="4" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
@@ -6426,13 +6426,13 @@
         <v>8</v>
       </c>
       <c r="C248" s="4" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="D248" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E248" s="4" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
@@ -6443,13 +6443,13 @@
         <v>8</v>
       </c>
       <c r="C249" s="4" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="D249" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E249" s="4" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
@@ -6460,13 +6460,13 @@
         <v>8</v>
       </c>
       <c r="C250" s="4" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="D250" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E250" s="4" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
@@ -6477,13 +6477,13 @@
         <v>137</v>
       </c>
       <c r="C251" s="4" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="D251" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E251" s="4" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
@@ -6494,13 +6494,13 @@
         <v>137</v>
       </c>
       <c r="C252" s="4" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="D252" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E252" s="4" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
@@ -6511,13 +6511,13 @@
         <v>137</v>
       </c>
       <c r="C253" s="4" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="D253" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E253" s="4" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
@@ -6528,13 +6528,13 @@
         <v>137</v>
       </c>
       <c r="C254" s="4" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="D254" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E254" s="4" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
@@ -6545,13 +6545,13 @@
         <v>137</v>
       </c>
       <c r="C255" s="4" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="D255" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E255" s="4" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
@@ -6562,13 +6562,13 @@
         <v>6</v>
       </c>
       <c r="C256" s="4" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="D256" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E256" s="4" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
@@ -6579,13 +6579,13 @@
         <v>6</v>
       </c>
       <c r="C257" s="4" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="D257" s="6" t="s">
-        <v>601</v>
+        <v>592</v>
       </c>
       <c r="E257" s="4" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
@@ -6596,13 +6596,13 @@
         <v>6</v>
       </c>
       <c r="C258" s="4" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="D258" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E258" s="4" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
@@ -6613,13 +6613,13 @@
         <v>6</v>
       </c>
       <c r="C259" s="4" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="D259" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E259" s="4" t="s">
-        <v>602</v>
+        <v>593</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
@@ -6630,13 +6630,13 @@
         <v>105</v>
       </c>
       <c r="C260" s="4" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="D260" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E260" s="4" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
@@ -6647,13 +6647,13 @@
         <v>6</v>
       </c>
       <c r="C261" s="4" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="D261" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E261" s="4" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
@@ -6664,13 +6664,13 @@
         <v>7</v>
       </c>
       <c r="C262" s="4" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="D262" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E262" s="4" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
@@ -6681,13 +6681,13 @@
         <v>7</v>
       </c>
       <c r="C263" s="4" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="D263" s="8">
         <v>3</v>
       </c>
       <c r="E263" s="4" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
@@ -6698,13 +6698,13 @@
         <v>7</v>
       </c>
       <c r="C264" s="4" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="D264" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E264" s="4" t="s">
-        <v>543</v>
+      <c r="E264" s="10" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
@@ -6715,13 +6715,13 @@
         <v>7</v>
       </c>
       <c r="C265" s="4" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="D265" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E265" s="4" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
@@ -6732,13 +6732,13 @@
         <v>7</v>
       </c>
       <c r="C266" s="4" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="D266" s="8">
         <v>3</v>
       </c>
       <c r="E266" s="4" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
@@ -6749,13 +6749,13 @@
         <v>7</v>
       </c>
       <c r="C267" s="4" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="D267" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E267" s="4" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
@@ -6766,13 +6766,13 @@
         <v>7</v>
       </c>
       <c r="C268" s="4" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="D268" s="8">
         <v>3</v>
       </c>
       <c r="E268" s="4" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
@@ -6783,13 +6783,13 @@
         <v>106</v>
       </c>
       <c r="C269" s="4" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="D269" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E269" s="4" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
@@ -6800,13 +6800,13 @@
         <v>7</v>
       </c>
       <c r="C270" s="4" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="D270" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E270" s="4" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
@@ -6817,13 +6817,13 @@
         <v>5</v>
       </c>
       <c r="C271" s="4" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="D271" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E271" s="4" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
@@ -6834,7 +6834,7 @@
         <v>5</v>
       </c>
       <c r="C272" s="4" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="D272" s="6" t="s">
         <v>13</v>
@@ -6851,7 +6851,7 @@
         <v>5</v>
       </c>
       <c r="C273" s="4" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="D273" s="6" t="s">
         <v>34</v>
@@ -6868,13 +6868,13 @@
         <v>5</v>
       </c>
       <c r="C274" s="4" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="D274" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E274" s="4" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
@@ -6885,7 +6885,7 @@
         <v>5</v>
       </c>
       <c r="C275" s="4" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="D275" s="6" t="s">
         <v>13</v>
@@ -6902,7 +6902,7 @@
         <v>5</v>
       </c>
       <c r="C276" s="4" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="D276" s="6" t="s">
         <v>34</v>
@@ -6919,13 +6919,13 @@
         <v>5</v>
       </c>
       <c r="C277" s="4" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="D277" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E277" s="4" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
@@ -6936,13 +6936,13 @@
         <v>5</v>
       </c>
       <c r="C278" s="4" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="D278" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E278" s="4" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
@@ -6952,14 +6952,14 @@
       <c r="B279" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="C279" s="4" t="s">
-        <v>568</v>
-      </c>
-      <c r="D279" s="6" t="s">
-        <v>34</v>
+      <c r="C279" s="10" t="s">
+        <v>608</v>
+      </c>
+      <c r="D279" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E279" s="4" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.25">
@@ -6970,13 +6970,13 @@
         <v>27</v>
       </c>
       <c r="C280" s="4" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="D280" s="6" t="s">
-        <v>601</v>
+        <v>592</v>
       </c>
       <c r="E280" s="4" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.25">
@@ -6987,13 +6987,13 @@
         <v>5</v>
       </c>
       <c r="C281" s="4" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="D281" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E281" s="4" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.25">
@@ -7004,13 +7004,13 @@
         <v>5</v>
       </c>
       <c r="C282" s="4" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="D282" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E282" s="4" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.25">
@@ -7021,13 +7021,13 @@
         <v>5</v>
       </c>
       <c r="C283" s="4" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="D283" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E283" s="4" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
@@ -7038,13 +7038,13 @@
         <v>5</v>
       </c>
       <c r="C284" s="4" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="D284" s="6" t="s">
-        <v>601</v>
+        <v>592</v>
       </c>
       <c r="E284" s="4" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.25">
@@ -7055,13 +7055,13 @@
         <v>216</v>
       </c>
       <c r="C285" s="4" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="D285" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E285" s="4" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
@@ -7072,13 +7072,13 @@
         <v>27</v>
       </c>
       <c r="C286" s="4" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="D286" s="6" t="s">
-        <v>601</v>
+        <v>592</v>
       </c>
       <c r="E286" s="4" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.25">
@@ -7089,13 +7089,13 @@
         <v>5</v>
       </c>
       <c r="C287" s="4" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
       <c r="D287" s="8">
         <v>3</v>
       </c>
       <c r="E287" s="4" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.25">
@@ -7106,13 +7106,13 @@
         <v>27</v>
       </c>
       <c r="C288" s="4" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="D288" s="8">
         <v>3</v>
       </c>
       <c r="E288" s="4" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.25">
@@ -7123,13 +7123,13 @@
         <v>27</v>
       </c>
       <c r="C289" s="4" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="D289" s="8">
         <v>3</v>
       </c>
       <c r="E289" s="4" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
@@ -7140,13 +7140,13 @@
         <v>216</v>
       </c>
       <c r="C290" s="4" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
       <c r="D290" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E290" s="4" t="s">
-        <v>591</v>
+      <c r="E290" s="10" t="s">
+        <v>609</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
@@ -7157,13 +7157,13 @@
         <v>216</v>
       </c>
       <c r="C291" s="4" t="s">
-        <v>592</v>
+        <v>585</v>
       </c>
       <c r="D291" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E291" s="4" t="s">
-        <v>593</v>
+      <c r="E291" s="10" t="s">
+        <v>610</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
@@ -7174,13 +7174,13 @@
         <v>216</v>
       </c>
       <c r="C292" s="4" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="D292" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E292" s="4" t="s">
-        <v>595</v>
+      <c r="E292" s="10" t="s">
+        <v>611</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
@@ -7191,13 +7191,13 @@
         <v>216</v>
       </c>
       <c r="C293" s="4" t="s">
-        <v>596</v>
+        <v>587</v>
       </c>
       <c r="D293" s="8">
         <v>3</v>
       </c>
       <c r="E293" s="4" t="s">
-        <v>597</v>
+        <v>588</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
@@ -7208,13 +7208,13 @@
         <v>216</v>
       </c>
       <c r="C294" s="4" t="s">
-        <v>598</v>
+        <v>589</v>
       </c>
       <c r="D294" s="8">
         <v>3</v>
       </c>
       <c r="E294" s="4" t="s">
-        <v>599</v>
+        <v>590</v>
       </c>
     </row>
   </sheetData>

</xml_diff>